<commit_message>
Adds OpenSeaDragon Live test of plate 11386
</commit_message>
<xml_diff>
--- a/excel-files/PlateBackgroundImageLinkMaker.xlsx
+++ b/excel-files/PlateBackgroundImageLinkMaker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Randel\source\repos\Galactic-Ping-Pong\excel-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2BD12A-11A1-4B43-80DC-8D98320F5214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FBF806-F426-4E84-B719-BEC0213AFDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4834BD2C-367E-44F7-81E1-CC9025577D13}"/>
+    <workbookView xWindow="1020" yWindow="570" windowWidth="27075" windowHeight="11385" xr2:uid="{4834BD2C-367E-44F7-81E1-CC9025577D13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7225646D-AFDF-4831-9CE4-41AD2AB32221}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,13 +543,13 @@
         <v>-4.5</v>
       </c>
       <c r="E2">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F2">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G2">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I2" t="str">
         <f>SUBSTITUTE(A2,"PlateCenterRA", C2)</f>
@@ -561,15 +561,15 @@
       </c>
       <c r="K2" t="str">
         <f>SUBSTITUTE(J2,"ImageScale",E2)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L2" t="str">
         <f>SUBSTITUTE(K2,"ImageWidth",F2)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M2" s="4" t="str">
         <f>SUBSTITUTE(L2,"ImageHeight",G2)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N2" s="5" t="str">
         <f>"PlateID-"&amp;B2&amp;".jpg"</f>
@@ -577,7 +577,7 @@
       </c>
       <c r="O2" s="1" t="str">
         <f>HYPERLINK(M2)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=37.25&amp;dec=-4.5&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -594,13 +594,13 @@
         <v>30.8125</v>
       </c>
       <c r="E3">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F3">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G3">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I45" si="0">SUBSTITUTE(A3,"PlateCenterRA", C3)</f>
@@ -612,15 +612,15 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K45" si="2">SUBSTITUTE(J3,"ImageScale",E3)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L45" si="3">SUBSTITUTE(K3,"ImageWidth",F3)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M3" s="4" t="str">
         <f t="shared" ref="M3:M45" si="4">SUBSTITUTE(L3,"ImageHeight",G3)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N3" s="5" t="str">
         <f t="shared" ref="N3:N45" si="5">"PlateID-"&amp;B3&amp;".jpg"</f>
@@ -628,7 +628,7 @@
       </c>
       <c r="O3" s="1" t="str">
         <f t="shared" ref="O3:O45" si="6">HYPERLINK(M3)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=148.311767578125&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -645,13 +645,13 @@
         <v>52.717830657958999</v>
       </c>
       <c r="E4">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F4">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G4">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -663,15 +663,15 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M4" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N4" s="5" t="str">
         <f t="shared" si="5"/>
@@ -679,7 +679,7 @@
       </c>
       <c r="O4" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=250.674957275391&amp;dec=52.717830657959&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -696,13 +696,13 @@
         <v>51.998153686523402</v>
       </c>
       <c r="E5">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F5">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G5">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -714,15 +714,15 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M5" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N5" s="5" t="str">
         <f t="shared" si="5"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="O5" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=193.654724121094&amp;dec=51.9981536865234&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -747,13 +747,13 @@
         <v>30.8125</v>
       </c>
       <c r="E6">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F6">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G6">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -765,15 +765,15 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M6" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N6" s="5" t="str">
         <f t="shared" si="5"/>
@@ -781,7 +781,7 @@
       </c>
       <c r="O6" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=143.561859130859&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>28.4375</v>
       </c>
       <c r="E7">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F7">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G7">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -816,15 +816,15 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M7" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N7" s="5" t="str">
         <f t="shared" si="5"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=168.498870849609&amp;dec=28.4375&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -849,13 +849,13 @@
         <v>24.400255203247099</v>
       </c>
       <c r="E8">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F8">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G8">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -867,15 +867,15 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M8" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N8" s="5" t="str">
         <f t="shared" si="5"/>
@@ -883,7 +883,7 @@
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=131.461578369141&amp;dec=24.4002552032471&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -900,13 +900,13 @@
         <v>25.139694213867202</v>
       </c>
       <c r="E9">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F9">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G9">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -918,15 +918,15 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M9" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N9" s="5" t="str">
         <f t="shared" si="5"/>
@@ -934,7 +934,7 @@
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=134.439208984375&amp;dec=25.1396942138672&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -951,13 +951,13 @@
         <v>44</v>
       </c>
       <c r="E10">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F10">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G10">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -969,15 +969,15 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M10" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N10" s="5" t="str">
         <f t="shared" si="5"/>
@@ -985,7 +985,7 @@
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=141.999984741211&amp;dec=44&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1002,13 +1002,13 @@
         <v>30.8125</v>
       </c>
       <c r="E11">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F11">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G11">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -1020,15 +1020,15 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M11" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N11" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="O11" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=160.1865234375&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1053,13 +1053,13 @@
         <v>30.8125</v>
       </c>
       <c r="E12">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F12">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G12">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -1071,15 +1071,15 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M12" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N12" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="O12" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=155.436630249023&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1104,13 +1104,13 @@
         <v>50.631587982177699</v>
       </c>
       <c r="E13">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F13">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G13">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -1122,15 +1122,15 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M13" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N13" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="O13" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=187.898544311523&amp;dec=50.6315879821777&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1155,13 +1155,13 @@
         <v>26.489660263061499</v>
       </c>
       <c r="E14">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F14">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G14">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -1173,15 +1173,15 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M14" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N14" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="O14" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=122.320281982422&amp;dec=26.4896602630615&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1206,13 +1206,13 @@
         <v>17.041233062744102</v>
       </c>
       <c r="E15">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F15">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G15">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -1224,15 +1224,15 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M15" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N15" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="O15" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.229133605957&amp;dec=17.0412330627441&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1257,13 +1257,13 @@
         <v>22.972883224487301</v>
       </c>
       <c r="E16">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F16">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G16">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -1275,15 +1275,15 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M16" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N16" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="O16" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=116.382461547852&amp;dec=22.9728832244873&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1308,13 +1308,13 @@
         <v>50.462917327880902</v>
       </c>
       <c r="E17">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F17">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G17">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -1326,15 +1326,15 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M17" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N17" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="O17" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=203.76399230957&amp;dec=50.4629173278809&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1359,13 +1359,13 @@
         <v>25.295284271240199</v>
       </c>
       <c r="E18">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F18">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G18">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
@@ -1377,15 +1377,15 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M18" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N18" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="O18" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=117.037200927734&amp;dec=25.2952842712402&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1410,13 +1410,13 @@
         <v>55.391849517822301</v>
       </c>
       <c r="E19">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F19">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G19">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
@@ -1428,15 +1428,15 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M19" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N19" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="O19" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=176.369323730469&amp;dec=55.3918495178223&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1461,13 +1461,13 @@
         <v>26.234308242797901</v>
       </c>
       <c r="E20">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F20">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G20">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -1479,15 +1479,15 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M20" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N20" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="O20" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=352.181243896484&amp;dec=26.2343082427979&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1512,13 +1512,13 @@
         <v>30.8125</v>
       </c>
       <c r="E21">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F21">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G21">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
@@ -1530,15 +1530,15 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M21" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N21" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="O21" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=186.311004638672&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1563,13 +1563,13 @@
         <v>46</v>
       </c>
       <c r="E22">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F22">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G22">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -1581,15 +1581,15 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M22" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N22" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="O22" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=115.300003051758&amp;dec=46&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1614,13 +1614,13 @@
         <v>33.228706359863303</v>
       </c>
       <c r="E23">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F23">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G23">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -1632,15 +1632,15 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M23" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N23" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="O23" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=166.765289306641&amp;dec=33.2287063598633&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1665,13 +1665,13 @@
         <v>51.399581909179702</v>
       </c>
       <c r="E24">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F24">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G24">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -1683,15 +1683,15 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M24" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N24" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="O24" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=248.123199462891&amp;dec=51.3995819091797&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1716,13 +1716,13 @@
         <v>30.8125</v>
       </c>
       <c r="E25">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F25">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G25">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
@@ -1734,15 +1734,15 @@
       </c>
       <c r="K25" t="str">
         <f>SUBSTITUTE(J25,"ImageScale",E25)</f>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M25" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N25" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="O25" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=167.311386108398&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1767,13 +1767,13 @@
         <v>16.6491813659668</v>
       </c>
       <c r="E26">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F26">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G26">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -1785,15 +1785,15 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M26" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N26" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="O26" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=27.4838771820068&amp;dec=16.6491813659668&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1818,13 +1818,13 @@
         <v>26.470821380615199</v>
       </c>
       <c r="E27">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F27">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G27">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -1836,15 +1836,15 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M27" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N27" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="O27" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=132.435150146484&amp;dec=26.4708213806152&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1869,13 +1869,13 @@
         <v>20.689975738525401</v>
       </c>
       <c r="E28">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F28">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G28">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
@@ -1887,15 +1887,15 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M28" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N28" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="O28" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=30.3078441619873&amp;dec=20.6899757385254&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1920,13 +1920,13 @@
         <v>30.8125</v>
       </c>
       <c r="E29">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F29">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G29">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -1938,15 +1938,15 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M29" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N29" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="O29" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=164.936431884766&amp;dec=30.8125&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F30">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G30">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
@@ -1980,15 +1980,15 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M30" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N30" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="O30" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2004,13 +2004,13 @@
         <v>3</v>
       </c>
       <c r="E31">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F31">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G31">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
@@ -2022,15 +2022,15 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M31" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N31" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="O31" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2046,13 +2046,13 @@
         <v>3</v>
       </c>
       <c r="E32">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F32">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G32">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -2064,15 +2064,15 @@
       </c>
       <c r="K32" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M32" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N32" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="O32" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2088,13 +2088,13 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F33">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G33">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="0"/>
@@ -2106,15 +2106,15 @@
       </c>
       <c r="K33" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M33" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N33" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="O33" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -2130,13 +2130,13 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F34">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G34">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
@@ -2148,15 +2148,15 @@
       </c>
       <c r="K34" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M34" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N34" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="O34" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -2172,13 +2172,13 @@
         <v>3</v>
       </c>
       <c r="E35">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F35">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G35">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
@@ -2190,15 +2190,15 @@
       </c>
       <c r="K35" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M35" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N35" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="O35" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -2214,13 +2214,13 @@
         <v>3</v>
       </c>
       <c r="E36">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F36">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G36">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="0"/>
@@ -2232,15 +2232,15 @@
       </c>
       <c r="K36" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M36" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N36" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="O36" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2256,13 +2256,13 @@
         <v>3</v>
       </c>
       <c r="E37">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F37">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G37">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="0"/>
@@ -2274,15 +2274,15 @@
       </c>
       <c r="K37" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M37" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N37" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="O37" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -2298,13 +2298,13 @@
         <v>3</v>
       </c>
       <c r="E38">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F38">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G38">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="0"/>
@@ -2316,15 +2316,15 @@
       </c>
       <c r="K38" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M38" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N38" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="O38" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -2340,13 +2340,13 @@
         <v>3</v>
       </c>
       <c r="E39">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F39">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G39">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="0"/>
@@ -2358,15 +2358,15 @@
       </c>
       <c r="K39" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M39" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N39" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="O39" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -2382,13 +2382,13 @@
         <v>3</v>
       </c>
       <c r="E40">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F40">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G40">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="0"/>
@@ -2400,15 +2400,15 @@
       </c>
       <c r="K40" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M40" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N40" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="O40" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -2424,13 +2424,13 @@
         <v>3</v>
       </c>
       <c r="E41">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F41">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G41">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="0"/>
@@ -2442,15 +2442,15 @@
       </c>
       <c r="K41" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M41" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N41" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="O41" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -2466,13 +2466,13 @@
         <v>3</v>
       </c>
       <c r="E42">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F42">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G42">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="0"/>
@@ -2484,15 +2484,15 @@
       </c>
       <c r="K42" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M42" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N42" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="O42" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -2508,13 +2508,13 @@
         <v>3</v>
       </c>
       <c r="E43">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F43">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G43">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="0"/>
@@ -2526,15 +2526,15 @@
       </c>
       <c r="K43" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M43" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N43" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="O43" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -2550,13 +2550,13 @@
         <v>3</v>
       </c>
       <c r="E44">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F44">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G44">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="0"/>
@@ -2568,15 +2568,15 @@
       </c>
       <c r="K44" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M44" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N44" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="O44" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2592,13 +2592,13 @@
         <v>3</v>
       </c>
       <c r="E45">
-        <v>15.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F45">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="G45">
-        <v>1080</v>
+        <v>2048</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="0"/>
@@ -2610,15 +2610,15 @@
       </c>
       <c r="K45" t="str">
         <f t="shared" si="2"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=ImageWidth&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=ImageWidth&amp;height=ImageHeight</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" si="3"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=ImageHeight</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=ImageHeight</v>
       </c>
       <c r="M45" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
       <c r="N45" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="O45" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=15.3&amp;width=1080&amp;height=1080</v>
+        <v>https://skyserver.sdss.org/dr17/Home/PrintChart?ra=&amp;dec=&amp;scale=8.05&amp;width=2048&amp;height=2048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>